<commit_message>
Fixed review input. Changed the way the log function is called. Variables names have changed based on input.
</commit_message>
<xml_diff>
--- a/tests/valid-testdata/Gis_map.xlsx
+++ b/tests/valid-testdata/Gis_map.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energinet-my.sharepoint.com/personal/tsp_energinet_dk/Documents/Dokumenter/Private Data/Projekter/DLR/Ny test data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E26BB4A-A8E2-4B47-A342-D70E6CB37697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{3E26BB4A-A8E2-4B47-A342-D70E6CB37697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B65A58F9-F691-4E84-A8FF-F42961954CB2}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{41B1FB18-306B-4EFD-A578-3E4E8259AA0E}"/>
+    <workbookView xWindow="45375" yWindow="5025" windowWidth="28800" windowHeight="15435" xr2:uid="{41B1FB18-306B-4EFD-A578-3E4E8259AA0E}"/>
   </bookViews>
   <sheets>
     <sheet name="GisMapping" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GisMapping!$A$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,19 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>GIS Name</t>
-  </si>
-  <si>
-    <t>ETS Name</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>E_ESK-MAV</t>
   </si>
@@ -59,14 +50,43 @@
   </si>
   <si>
     <t>E_BLA-MAV</t>
+  </si>
+  <si>
+    <t>Andet navn i ETS</t>
+  </si>
+  <si>
+    <t>Andet navn i GIS</t>
+  </si>
+  <si>
+    <t>TSP</t>
+  </si>
+  <si>
+    <t>ETS LINE NAME</t>
+  </si>
+  <si>
+    <t>GIS LINE NAME</t>
+  </si>
+  <si>
+    <t>COMMENT</t>
+  </si>
+  <si>
+    <t>USER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -94,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,47 +434,60 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{8715D4FF-12CA-4C4C-AC70-C5BAEB7C3CE5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>